<commit_message>
More setup of the independent measures scripts
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -139,28 +139,6 @@
           </rPr>
           <t xml:space="preserve">
 All data, or only matched notifications/contracts</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Shaun McGirr:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Is this measuring something that should strictly never happen? Or measure something that is unusual? Ie bunching at thresholds is just unusual, not illegal</t>
         </r>
       </text>
     </comment>
@@ -182,7 +160,74 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
+Is this measuring something that should strictly never happen? Or measure something that is unusual? Ie bunching at thresholds is just unusual, not illegal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
 R script that builds the measure</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+English: http://en.fas.gov.ru/documents/documentdetails.html?id=13920
+Russian: http://fas.gov.ru/documents/documentdetails.html?id=13</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+http://www.againstcorruption.eu/reports/uncovering-high-level-corruption/ </t>
         </r>
       </text>
     </comment>
@@ -191,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>MeasureName</t>
   </si>
@@ -245,6 +290,84 @@
   </si>
   <si>
     <t>contracts-not-notified.R</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Median price change</t>
+  </si>
+  <si>
+    <t>Mean price change</t>
+  </si>
+  <si>
+    <t>Median of the percentage price change between notification and contract (outliers excluded)</t>
+  </si>
+  <si>
+    <t>Mean of the percentage price change between notification and contract (outliers excluded)</t>
+  </si>
+  <si>
+    <t>During</t>
+  </si>
+  <si>
+    <t>Balsevich 2014</t>
+  </si>
+  <si>
+    <t>Matched only</t>
+  </si>
+  <si>
+    <t>ByDimensions</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Month, Procedure</t>
+  </si>
+  <si>
+    <t>Median of (-1*(notification price - contract price))/notification price)*100, excluding changes over 100%</t>
+  </si>
+  <si>
+    <t>Mean of (-1*(notification price - contract price))/notification price)*100, excluding changes over 100%</t>
+  </si>
+  <si>
+    <t>Corruption less likely with larger change during procedure</t>
+  </si>
+  <si>
+    <t>price-changes.R</t>
+  </si>
+  <si>
+    <t>Repeat winners (number)</t>
+  </si>
+  <si>
+    <t>Repeat winners (value)</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts awarded to most-winning supplier</t>
+  </si>
+  <si>
+    <t>Proportion of spending by agency awarded to most-winning supplier</t>
+  </si>
+  <si>
+    <t>Fazekas &amp; Kocsis 2015</t>
+  </si>
+  <si>
+    <t>Candidates</t>
+  </si>
+  <si>
+    <t>Fiddling with open tender</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%9E%D1%82%D0%BA%D1%80%D1%8B%D1%82%D1%8B%D0%B9_%D0%BA%D0%BE%D0%BD%D0%BA%D1%83%D1%80%D1%81</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>https://clearspending.ru/in-control/</t>
   </si>
 </sst>
 </file>
@@ -585,28 +708,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="34.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -625,17 +750,23 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -654,14 +785,130 @@
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing location of non-Git data downloads
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -231,12 +231,59 @@
         </r>
       </text>
     </comment>
+    <comment ref="E7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+  # Turns out the notifications with a matching contract, but where many contract details NA, are interesting
+  # eg http://zakupki.gov.ru/pgz/public/action/orders/info/common_info/show?notificationId=7443504 (contract not linked)
+  # eg http://zakupki.gov.ru/pgz/public/action/orders/info/common_info/show?notificationId=7598466 (contract 'there' but not)
+  # Perhaps these should be measures? Provisionally, treat any final data quality issues as potential measures</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Dominant procedure?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>MeasureName</t>
   </si>
@@ -368,6 +415,143 @@
   </si>
   <si>
     <t>https://clearspending.ru/in-control/</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts with substantially missing details</t>
+  </si>
+  <si>
+    <t>See comment</t>
+  </si>
+  <si>
+    <t>Contract details missing</t>
+  </si>
+  <si>
+    <t>Notification revisions</t>
+  </si>
+  <si>
+    <t>Contract revisions</t>
+  </si>
+  <si>
+    <t>Mean number of agency revisions to notifications</t>
+  </si>
+  <si>
+    <t>Mean number of agency revisions to contracts</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Total agency spend</t>
+  </si>
+  <si>
+    <t>Total spent by agency</t>
+  </si>
+  <si>
+    <t>Sum of ContractPrice by agency</t>
+  </si>
+  <si>
+    <t>Provisionally, treat any final data quality issues as potential measures</t>
+  </si>
+  <si>
+    <t>Control variable</t>
+  </si>
+  <si>
+    <t>Listing duration</t>
+  </si>
+  <si>
+    <t>ContractSignDate - NotificationPublishDate</t>
+  </si>
+  <si>
+    <t>Mean days notification is listed before awarding contract</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts awarded after price change &gt;15%</t>
+  </si>
+  <si>
+    <t>Count of contracts where (contract price - notification price)/notification price exceeds 15%</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Dramatic price drop from notification to contract - indicates risk of 'cheap analogue' being supplied
+    #   - a valid measure because FL-44 prevented it in cases more than 15% without contract explaining why
+    #   - concrete case https://www.hse.ru/pubs/share/direct/document/64729394</t>
+  </si>
+  <si>
+    <t>Median number of bidders per purchase notified</t>
+  </si>
+  <si>
+    <t>Bidders per notification</t>
+  </si>
+  <si>
+    <t>Dramatic price drop</t>
+  </si>
+  <si>
+    <t>Dramatic price increase</t>
+  </si>
+  <si>
+    <t>Discontinuity at price increase of 10/100% could indicate gaming</t>
+  </si>
+  <si>
+    <t>Proportion of contracts near 10% and 100% over notified value</t>
+  </si>
+  <si>
+    <t>Change of product</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts where notification product code is not contract product code</t>
+  </si>
+  <si>
+    <t>Changes correlated with fiddling</t>
+  </si>
+  <si>
+    <t>Less auditable quantities</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts where non-countable quantity used</t>
+  </si>
+  <si>
+    <t>Buying "1 piece" of road is less transparent than buying X miles</t>
+  </si>
+  <si>
+    <t>Listing irregularities</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts listed near procedure threshold</t>
+  </si>
+  <si>
+    <t>Clear evidence of gaming when so many listed right below 500,000</t>
+  </si>
+  <si>
+    <t>Proportion of contracts within 1% of relevant threshold</t>
+  </si>
+  <si>
+    <t>Fewer bidders increases risk (correlated with weaker market and with disqualifications)</t>
+  </si>
+  <si>
+    <t>Procedure choice</t>
+  </si>
+  <si>
+    <t>Summary measure possible?</t>
+  </si>
+  <si>
+    <t>Independent variable</t>
+  </si>
+  <si>
+    <t>Is this correlated with specificity?</t>
+  </si>
+  <si>
+    <t>Purchase specificity (count)</t>
+  </si>
+  <si>
+    <t>Purchase specificity (value)</t>
+  </si>
+  <si>
+    <t>Deviation from average proportion spent by agency per product</t>
+  </si>
+  <si>
+    <t>Number of products not purchased by any other agency</t>
   </si>
 </sst>
 </file>
@@ -708,18 +892,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
@@ -890,24 +1074,262 @@
         <v>37</v>
       </c>
     </row>
+    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="25" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moving calculations of measures based on single products to standalone file
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -283,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
   <si>
     <t>MeasureName</t>
   </si>
@@ -552,6 +552,36 @@
   </si>
   <si>
     <t>Number of products not purchased by any other agency</t>
+  </si>
+  <si>
+    <t>Low-efficiency auctions</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts awarded where price change &lt;1%</t>
+  </si>
+  <si>
+    <t>Preponderance of auctions in this band difficult to justify</t>
+  </si>
+  <si>
+    <t>Nested agencies</t>
+  </si>
+  <si>
+    <t>"turtles all the way down"</t>
+  </si>
+  <si>
+    <t>My theory should apply within as across agencies. The actors are just junior and senior so we should see same patterns "zooming in" on agencies</t>
+  </si>
+  <si>
+    <t>Is it possible to identify these measures within agences? Perhaps agency names within regnum? Or use different budget sources?</t>
+  </si>
+  <si>
+    <t>Regional vs Federal</t>
+  </si>
+  <si>
+    <t>Identifiable from ContractFinance fields</t>
+  </si>
+  <si>
+    <t>Are the corruption measures different out in regions based on whether funds are federal?</t>
   </si>
 </sst>
 </file>
@@ -892,13 +922,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,24 +1342,66 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="28" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changing labels on procedure usage graph and adding new graph of efficiency vs spend
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -256,28 +256,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Shaun McGirr:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Dominant procedure?</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -515,9 +493,6 @@
     <t>Buying "1 piece" of road is less transparent than buying X miles</t>
   </si>
   <si>
-    <t>Listing irregularities</t>
-  </si>
-  <si>
     <t>Proportion of agency contracts listed near procedure threshold</t>
   </si>
   <si>
@@ -530,12 +505,6 @@
     <t>Fewer bidders increases risk (correlated with weaker market and with disqualifications)</t>
   </si>
   <si>
-    <t>Procedure choice</t>
-  </si>
-  <si>
-    <t>Summary measure possible?</t>
-  </si>
-  <si>
     <t>Independent variable</t>
   </si>
   <si>
@@ -582,6 +551,15 @@
   </si>
   <si>
     <t>Are the corruption measures different out in regions based on whether funds are federal?</t>
+  </si>
+  <si>
+    <t>Dominant procedure</t>
+  </si>
+  <si>
+    <t>Agency uses one procedure for all purchases</t>
+  </si>
+  <si>
+    <t>Bunched listing prices</t>
   </si>
 </sst>
 </file>
@@ -925,10 +903,10 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1246,7 +1224,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1285,100 +1263,100 @@
     </row>
     <row r="17" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Drafting several 'red flag' measures
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
   <si>
     <t>MeasureName</t>
   </si>
@@ -318,9 +318,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Median price change</t>
@@ -560,6 +557,9 @@
   </si>
   <si>
     <t>Bunched listing prices</t>
+  </si>
+  <si>
+    <t>Draft</t>
   </si>
 </sst>
 </file>
@@ -903,10 +903,10 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -978,7 +978,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -990,266 +990,266 @@
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
       <c r="I7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1258,129 +1258,135 @@
         <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    </row>
+    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>85</v>
       </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I23" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding further measures of corruption
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
   <si>
     <t>MeasureName</t>
   </si>
@@ -463,15 +463,6 @@
     <t>Dramatic price drop</t>
   </si>
   <si>
-    <t>Dramatic price increase</t>
-  </si>
-  <si>
-    <t>Discontinuity at price increase of 10/100% could indicate gaming</t>
-  </si>
-  <si>
-    <t>Proportion of contracts near 10% and 100% over notified value</t>
-  </si>
-  <si>
     <t>Change of product</t>
   </si>
   <si>
@@ -560,13 +551,49 @@
   </si>
   <si>
     <t>Draft</t>
+  </si>
+  <si>
+    <t>&lt;protocolEF3&gt;</t>
+  </si>
+  <si>
+    <t>Need XML to simply count number of applications per lot</t>
+  </si>
+  <si>
+    <t>Would need to parse protocols, see eg 3-Unpack/example-of-protocols…</t>
+  </si>
+  <si>
+    <t>Agency wages</t>
+  </si>
+  <si>
+    <t>Median wage for bureaucrats in each agency</t>
+  </si>
+  <si>
+    <t>GKS (saved in data_other)</t>
+  </si>
+  <si>
+    <t>Read in directly from 2015 GKS data and matched to agency names</t>
+  </si>
+  <si>
+    <t>Single bidder</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts awarded when only one bidder</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>Price increase</t>
+  </si>
+  <si>
+    <t>Proportion of contracts where price increased</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -593,6 +620,14 @@
       <color indexed="81"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -611,10 +646,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -623,8 +659,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -900,13 +938,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,7 +1028,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1025,7 +1063,7 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1060,7 +1098,7 @@
         <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1073,6 +1111,9 @@
       <c r="E5" t="s">
         <v>37</v>
       </c>
+      <c r="K5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1112,6 +1153,9 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
+      <c r="K8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1126,6 +1170,9 @@
       <c r="D9" t="s">
         <v>50</v>
       </c>
+      <c r="K9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1192,13 +1239,16 @@
       <c r="I12" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="K12" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1206,8 +1256,8 @@
       <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>67</v>
+      <c r="K13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1218,179 +1268,223 @@
         <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
       </c>
+      <c r="E14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="I14" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>77</v>
+      <c r="D17" t="s">
+        <v>12</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" t="s">
         <v>95</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    </row>
+    <row r="23" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="24" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding ideas for measures
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -256,12 +256,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="E29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Shaun McGirr:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Unusual bid patterns.  For example, the bids are:
+Too high
+Too close
+Too consistent
+Too far apart
+Round numbers
+Incomplete Identical or similar to prior or other bid</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="139">
   <si>
     <t>MeasureName</t>
   </si>
@@ -587,6 +615,99 @@
   </si>
   <si>
     <t>Proportion of contracts where price increased</t>
+  </si>
+  <si>
+    <t>As explained in World Bank 'red flags' doc</t>
+  </si>
+  <si>
+    <t>Unusual bidding patterns</t>
+  </si>
+  <si>
+    <t>More implies collusion among bidders, not necessarily fiddling by bureaucrats</t>
+  </si>
+  <si>
+    <t>Draft - not used</t>
+  </si>
+  <si>
+    <t>Product substitution</t>
+  </si>
+  <si>
+    <t>Unobservable</t>
+  </si>
+  <si>
+    <t>World Bank</t>
+  </si>
+  <si>
+    <t>Contract price increase</t>
+  </si>
+  <si>
+    <t>Increase in price of contract over several versions</t>
+  </si>
+  <si>
+    <t>Would need to re-parse contracts in the de-duplication stage</t>
+  </si>
+  <si>
+    <t>Multiple ways to measure irregularities in bidding</t>
+  </si>
+  <si>
+    <t>Need to parse protocols first</t>
+  </si>
+  <si>
+    <t>Could probably identify these</t>
+  </si>
+  <si>
+    <t>Strange assessment criteria</t>
+  </si>
+  <si>
+    <t>Single supplier reasons</t>
+  </si>
+  <si>
+    <t>Unnecessary purchases</t>
+  </si>
+  <si>
+    <t>Unusual or unexplained high volume purchases of products or services from a particular supplier</t>
+  </si>
+  <si>
+    <t>IACRC</t>
+  </si>
+  <si>
+    <t>A better version of market share measures?</t>
+  </si>
+  <si>
+    <t>Sole source award above or just below competitive bidding limits</t>
+  </si>
+  <si>
+    <t>Price distribution of single supplier</t>
+  </si>
+  <si>
+    <t>Split purchases</t>
+  </si>
+  <si>
+    <t>Similar auctions together very close in time</t>
+  </si>
+  <si>
+    <t>Bid proximity</t>
+  </si>
+  <si>
+    <t>In request for quotes (sealed-bid), suspicious if winning bid only slightly lower then 2nd-place</t>
+  </si>
+  <si>
+    <t>Sealed-bid auction info leaked</t>
+  </si>
+  <si>
+    <t>Bid timing</t>
+  </si>
+  <si>
+    <t>Late bidder is lowest bidder</t>
+  </si>
+  <si>
+    <t>Don't expect correlation</t>
+  </si>
+  <si>
+    <t>World Bank, IACRC</t>
+  </si>
+  <si>
+    <t>Collusive bidding</t>
   </si>
 </sst>
 </file>
@@ -629,12 +750,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -650,7 +777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -660,6 +787,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,13 +1072,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,6 +1256,9 @@
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1154,7 +1291,7 @@
         <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1171,44 +1308,35 @@
         <v>50</v>
       </c>
       <c r="K9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>28</v>
@@ -1216,13 +1344,16 @@
       <c r="I11" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1231,24 +1362,24 @@
         <v>50</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1256,139 +1387,148 @@
       <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="K13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>105</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>74</v>
+      <c r="D18" t="s">
+        <v>12</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I19" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="K19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1400,91 +1540,243 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="26" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E25" r:id="rId1"/>
+    <hyperlink ref="E26" r:id="rId1"/>
+    <hyperlink ref="E32" r:id="rId2"/>
+    <hyperlink ref="E33" r:id="rId3"/>
+    <hyperlink ref="E34" r:id="rId4"/>
+    <hyperlink ref="E35" r:id="rId5"/>
+    <hyperlink ref="E36" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Herfindahl index to measure winner concentration
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -231,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -256,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E29" authorId="0">
+    <comment ref="E30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
   <si>
     <t>MeasureName</t>
   </si>
@@ -708,6 +708,15 @@
   </si>
   <si>
     <t>Collusive bidding</t>
+  </si>
+  <si>
+    <t>Winner concentration</t>
+  </si>
+  <si>
+    <t>Herfindahl-Hirschman index of winners' share of agency budget</t>
+  </si>
+  <si>
+    <t>Anti-trust literature</t>
   </si>
 </sst>
 </file>
@@ -1072,13 +1081,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1246,7 +1255,7 @@
         <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1257,55 +1266,52 @@
         <v>36</v>
       </c>
       <c r="K6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" t="s">
-        <v>111</v>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="K9" t="s">
         <v>111</v>
@@ -1313,56 +1319,47 @@
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>28</v>
@@ -1374,12 +1371,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1388,24 +1385,24 @@
         <v>50</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1413,139 +1410,148 @@
       <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="K14" t="s">
+      <c r="F14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>105</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>74</v>
+      <c r="D19" t="s">
+        <v>12</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
+      <c r="F20" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I20" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="K20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1557,224 +1563,241 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="I23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>112</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="I33" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>129</v>
+      <c r="A34" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>131</v>
+    <row r="35" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>125</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E39" s="3"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E26" r:id="rId1"/>
-    <hyperlink ref="E32" r:id="rId2"/>
-    <hyperlink ref="E33" r:id="rId3"/>
-    <hyperlink ref="E34" r:id="rId4"/>
-    <hyperlink ref="E35" r:id="rId5"/>
-    <hyperlink ref="E36" r:id="rId6"/>
+    <hyperlink ref="E27" r:id="rId1"/>
+    <hyperlink ref="E33" r:id="rId2"/>
+    <hyperlink ref="E34" r:id="rId3"/>
+    <hyperlink ref="E35" r:id="rId4"/>
+    <hyperlink ref="E36" r:id="rId5"/>
+    <hyperlink ref="E37" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId7"/>

</xml_diff>

<commit_message>
Adding code to compare to NRPZ measure
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="146">
   <si>
     <t>MeasureName</t>
   </si>
@@ -717,6 +717,18 @@
   </si>
   <si>
     <t>Anti-trust literature</t>
+  </si>
+  <si>
+    <t>Audit chamber enquiries</t>
+  </si>
+  <si>
+    <t>Number of enquiries</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>The Audit Chamber, the main oversight agency of the Executive, releases yearly reports on its activities, including the number of inquiries initiated in to each agency, and the `yield' of these inquiries in terms of cases forwarded to prosecutors.</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1096,10 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1757,8 +1769,19 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E38" s="5"/>
+    <row r="38" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E39" s="5"/>

</xml_diff>

<commit_message>
Minor tweaks to GCB plots for chapter 1 based on Allen's comments
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
   <si>
     <t>MeasureName</t>
   </si>
@@ -587,9 +587,6 @@
     <t>Need XML to simply count number of applications per lot</t>
   </si>
   <si>
-    <t>Would need to parse protocols, see eg 3-Unpack/example-of-protocols…</t>
-  </si>
-  <si>
     <t>Agency wages</t>
   </si>
   <si>
@@ -729,6 +726,28 @@
   </si>
   <si>
     <t>The Audit Chamber, the main oversight agency of the Executive, releases yearly reports on its activities, including the number of inquiries initiated in to each agency, and the `yield' of these inquiries in terms of cases forwarded to prosecutors.</t>
+  </si>
+  <si>
+    <t>Bunching at time points</t>
+  </si>
+  <si>
+    <t>Bunching at cutoffs and nice round numbers are clear, looking at dates should be just as useful</t>
+  </si>
+  <si>
+    <t>Brian had the idea to look at purchasing over, time is there a rush to spend near end of year? (although this happens always)</t>
+  </si>
+  <si>
+    <t>Round number prices</t>
+  </si>
+  <si>
+    <t>On both the listing and contract side</t>
+  </si>
+  <si>
+    <t>Proportion of agency contracts listed/awarded at round number</t>
+  </si>
+  <si>
+    <t>Would need to parse protocols, see eg 3-Unpack/example-of-protocols…
+Very important for efficiency story</t>
   </si>
 </sst>
 </file>
@@ -1093,13 +1112,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1286,7 @@
         <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1278,18 +1297,18 @@
         <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="E7" t="s">
         <v>140</v>
-      </c>
-      <c r="E7" t="s">
-        <v>141</v>
       </c>
       <c r="K7" t="s">
         <v>95</v>
@@ -1326,7 +1345,7 @@
         <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1343,21 +1362,21 @@
         <v>50</v>
       </c>
       <c r="K10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="E11" t="s">
-        <v>114</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1437,10 +1456,10 @@
     </row>
     <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1460,7 +1479,7 @@
         <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -1469,7 +1488,7 @@
         <v>96</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>75</v>
@@ -1480,10 +1499,10 @@
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1636,16 +1655,16 @@
     </row>
     <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="E27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>55</v>
@@ -1653,163 +1672,184 @@
     </row>
     <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="E33" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="I33" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="E35" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="E36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="E37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="E38" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="F38" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F38" s="3" t="s">
+    </row>
+    <row r="39" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F39" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding purchase-level tests to back up agency-level analysis
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -256,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E30" authorId="0">
+    <comment ref="E31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="155">
   <si>
     <t>MeasureName</t>
   </si>
@@ -748,6 +748,15 @@
   <si>
     <t>Would need to parse protocols, see eg 3-Unpack/example-of-protocols…
 Very important for efficiency story</t>
+  </si>
+  <si>
+    <t>Agency, Purchase</t>
+  </si>
+  <si>
+    <t>Purchase specificity (probability</t>
+  </si>
+  <si>
+    <t>Probability that a purchase is from the given product category</t>
   </si>
 </sst>
 </file>
@@ -817,7 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -831,9 +840,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1112,13 +1122,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1282,6 +1292,9 @@
       <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
@@ -1307,6 +1320,9 @@
       <c r="B7" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
       <c r="E7" t="s">
         <v>140</v>
       </c>
@@ -1339,7 +1355,7 @@
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -1356,7 +1372,7 @@
         <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
         <v>50</v>
@@ -1410,7 +1426,7 @@
         <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
         <v>50</v>
@@ -1505,7 +1521,7 @@
         <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -1517,7 +1533,7 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
         <v>50</v>
@@ -1534,7 +1550,7 @@
         <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1551,7 +1567,7 @@
         <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>74</v>
@@ -1613,254 +1629,283 @@
     </row>
     <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="K25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>111</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>113</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>119</v>
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>122</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>124</v>
       </c>
+      <c r="I34" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>128</v>
+      <c r="A35" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>130</v>
+    <row r="36" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>133</v>
+    </row>
+    <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>124</v>
       </c>
       <c r="I37" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="112" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>141</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="3" t="s">
+      <c r="E40" s="5"/>
+      <c r="F40" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1"/>
-    <hyperlink ref="E33" r:id="rId2"/>
-    <hyperlink ref="E34" r:id="rId3"/>
-    <hyperlink ref="E35" r:id="rId4"/>
-    <hyperlink ref="E36" r:id="rId5"/>
-    <hyperlink ref="E37" r:id="rId6"/>
+    <hyperlink ref="E28" r:id="rId1"/>
+    <hyperlink ref="E34" r:id="rId2"/>
+    <hyperlink ref="E35" r:id="rId3"/>
+    <hyperlink ref="E36" r:id="rId4"/>
+    <hyperlink ref="E37" r:id="rId5"/>
+    <hyperlink ref="E38" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId7"/>

</xml_diff>

<commit_message>
Commiting script to extract bid information with both approaches showing
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="158">
   <si>
     <t>MeasureName</t>
   </si>
@@ -757,6 +757,15 @@
   </si>
   <si>
     <t>Probability that a purchase is from the given product category</t>
+  </si>
+  <si>
+    <t>Alternative explanation is too easy: "we're just lazy"</t>
+  </si>
+  <si>
+    <t>Can't get this from my data</t>
+  </si>
+  <si>
+    <t>Draft - better at purchase level</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1134,10 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,6 +1152,7 @@
     <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1176,7 +1186,7 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1246,7 +1256,7 @@
       <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1281,25 +1291,25 @@
       <c r="J4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="K5" t="s">
-        <v>110</v>
+      <c r="K5" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1309,7 +1319,7 @@
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1326,7 +1336,7 @@
       <c r="E7" t="s">
         <v>140</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1360,7 +1370,7 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1377,7 +1387,7 @@
       <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1444,7 +1454,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1483,7 +1493,7 @@
       <c r="D15" t="s">
         <v>50</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1514,7 +1524,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1575,7 +1585,7 @@
       <c r="I20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1606,7 +1616,7 @@
       <c r="I22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1623,7 +1633,7 @@
       <c r="I23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1640,7 +1650,7 @@
       <c r="I24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1657,7 +1667,7 @@
       <c r="I25" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1797,7 +1807,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="8" t="s">
         <v>130</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1809,12 +1819,15 @@
       <c r="E37" s="5" t="s">
         <v>124</v>
       </c>
+      <c r="H37" t="s">
+        <v>156</v>
+      </c>
       <c r="I37" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="8" t="s">
         <v>133</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1825,6 +1838,9 @@
       </c>
       <c r="E38" s="5" t="s">
         <v>124</v>
+      </c>
+      <c r="H38" t="s">
+        <v>156</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>135</v>
@@ -1857,7 +1873,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="8" t="s">
         <v>148</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -1869,6 +1885,9 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
         <v>149</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Shifting code to build favoritism measure to build-purchase-data
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="158">
   <si>
     <t>MeasureName</t>
   </si>
@@ -1134,10 +1134,10 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1498,7 +1498,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1522,9 +1522,12 @@
       <c r="J16" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="K16" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1534,6 +1537,9 @@
         <v>152</v>
       </c>
       <c r="J17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">

</xml_diff>

<commit_message>
Adding regional FE model and table of Moscow ministries
</commit_message>
<xml_diff>
--- a/4-Construct/measures/inventory-of-measures.xlsx
+++ b/4-Construct/measures/inventory-of-measures.xlsx
@@ -808,18 +808,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -835,7 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -848,7 +842,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1296,13 +1289,13 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>152</v>
       </c>
       <c r="E5" t="s">
@@ -1498,7 +1491,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1527,7 +1520,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1791,7 +1784,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>127</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1802,7 +1795,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>128</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1813,7 +1806,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1833,7 +1826,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1879,7 +1872,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B41" s="3" t="s">

</xml_diff>